<commit_message>
TDD: test2<Resource>EntityEffect (for lumber, clay, ore, stone) pass
</commit_message>
<xml_diff>
--- a/resources/Effects.xlsx
+++ b/resources/Effects.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="42">
   <si>
     <t xml:space="preserve">Effect</t>
   </si>
@@ -160,6 +160,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -182,12 +183,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -435,23 +438,23 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.1836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.47959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.0867346938776"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.3775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1386,8 +1389,12 @@
       <c r="B30" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
+      <c r="C30" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="13" t="s">
@@ -1411,8 +1418,12 @@
       <c r="B31" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
+      <c r="C31" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="13" t="s">
@@ -1436,8 +1447,12 @@
       <c r="B32" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
+      <c r="C32" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E32" s="12" t="n">
         <v>1</v>
       </c>
@@ -1465,7 +1480,9 @@
       <c r="B33" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="13"/>
+      <c r="C33" s="13" t="n">
+        <v>1</v>
+      </c>
       <c r="D33" s="14"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
@@ -1484,7 +1501,9 @@
       <c r="B34" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="13"/>
+      <c r="C34" s="13" t="n">
+        <v>1</v>
+      </c>
       <c r="D34" s="14"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
@@ -1503,7 +1522,9 @@
       <c r="B35" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="13"/>
+      <c r="C35" s="13" t="n">
+        <v>1</v>
+      </c>
       <c r="D35" s="14"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>

</xml_diff>

<commit_message>
TDD: test1<Science>EntityEffect (for protractor, wheel, and tablet) pass
</commit_message>
<xml_diff>
--- a/resources/Effects.xlsx
+++ b/resources/Effects.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="43">
   <si>
     <t xml:space="preserve">Effect</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">Guild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">Neighbors</t>
@@ -438,23 +441,19 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.5714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -735,7 +734,9 @@
       <c r="C9" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E9" s="12" t="n">
         <v>6</v>
       </c>
@@ -776,7 +777,9 @@
       <c r="C10" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="D10" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E10" s="12" t="n">
         <v>7</v>
       </c>
@@ -811,7 +814,9 @@
       <c r="C11" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="D11" s="14"/>
+      <c r="D11" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E11" s="12" t="n">
         <v>8</v>
       </c>
@@ -852,7 +857,9 @@
       <c r="C12" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E12" s="10" t="s">
         <v>24</v>
       </c>
@@ -881,7 +888,9 @@
       <c r="C13" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="14"/>
+      <c r="D13" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E13" s="12" t="n">
         <v>1</v>
       </c>
@@ -912,7 +921,9 @@
       <c r="C14" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E14" s="12" t="n">
         <v>2</v>
       </c>
@@ -939,7 +950,7 @@
         <v>16</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O14" s="14"/>
     </row>
@@ -953,7 +964,9 @@
       <c r="C15" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="14"/>
+      <c r="D15" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E15" s="12" t="n">
         <v>3</v>
       </c>
@@ -988,7 +1001,9 @@
       <c r="C16" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="14"/>
+      <c r="D16" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E16" s="15" t="s">
         <v>11</v>
       </c>
@@ -1013,7 +1028,9 @@
       <c r="C17" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="14"/>
+      <c r="D17" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E17" s="12" t="n">
         <v>1</v>
       </c>
@@ -1021,7 +1038,7 @@
         <v>17</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H17" s="13" t="s">
         <v>9</v>
@@ -1042,7 +1059,9 @@
       <c r="C18" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="14"/>
+      <c r="D18" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E18" s="12" t="n">
         <v>1</v>
       </c>
@@ -1050,7 +1069,7 @@
         <v>17</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H18" s="13" t="s">
         <v>9</v>
@@ -1073,7 +1092,9 @@
       <c r="C19" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="14"/>
+      <c r="D19" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E19" s="12" t="n">
         <v>1</v>
       </c>
@@ -1081,7 +1102,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>9</v>
@@ -1102,7 +1123,9 @@
       <c r="C20" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="14"/>
+      <c r="D20" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E20" s="12" t="n">
         <v>1</v>
       </c>
@@ -1110,7 +1133,7 @@
         <v>17</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H20" s="13" t="s">
         <v>20</v>
@@ -1133,7 +1156,9 @@
       <c r="C21" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="14"/>
+      <c r="D21" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E21" s="12" t="n">
         <v>1</v>
       </c>
@@ -1141,7 +1166,7 @@
         <v>17</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H21" s="13" t="s">
         <v>20</v>
@@ -1162,7 +1187,9 @@
       <c r="C22" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="14"/>
+      <c r="D22" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E22" s="10" t="s">
         <v>26</v>
       </c>
@@ -1187,7 +1214,9 @@
       <c r="C23" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="14"/>
+      <c r="D23" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E23" s="12" t="n">
         <v>1</v>
       </c>
@@ -1195,7 +1224,7 @@
         <v>14</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>9</v>
@@ -1216,7 +1245,9 @@
       <c r="C24" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D24" s="14"/>
+      <c r="D24" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E24" s="12" t="n">
         <v>2</v>
       </c>
@@ -1224,7 +1255,7 @@
         <v>14</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>20</v>
@@ -1247,7 +1278,9 @@
       <c r="C25" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="14"/>
+      <c r="D25" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E25" s="12" t="n">
         <v>1</v>
       </c>
@@ -1255,7 +1288,7 @@
         <v>14</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H25" s="13" t="s">
         <v>22</v>
@@ -1276,7 +1309,9 @@
       <c r="C26" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="14"/>
+      <c r="D26" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E26" s="12" t="n">
         <v>1</v>
       </c>
@@ -1284,10 +1319,10 @@
         <v>14</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I26" s="14"/>
       <c r="J26" s="13"/>
@@ -1305,7 +1340,9 @@
       <c r="C27" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="14"/>
+      <c r="D27" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E27" s="12" t="n">
         <v>1</v>
       </c>
@@ -1313,10 +1350,10 @@
         <v>14</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I27" s="14"/>
       <c r="J27" s="13"/>
@@ -1334,7 +1371,9 @@
       <c r="C28" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D28" s="14"/>
+      <c r="D28" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E28" s="12" t="n">
         <v>1</v>
       </c>
@@ -1342,10 +1381,10 @@
         <v>14</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I28" s="14"/>
       <c r="J28" s="13"/>
@@ -1387,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C30" s="13" t="n">
         <v>1</v>
@@ -1416,7 +1455,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C31" s="13" t="n">
         <v>1</v>
@@ -1430,7 +1469,7 @@
         <v>15</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I31" s="14"/>
       <c r="J31" s="13"/>
@@ -1445,7 +1484,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C32" s="13" t="n">
         <v>1</v>
@@ -1460,7 +1499,7 @@
         <v>14</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H32" s="13" t="s">
         <v>23</v>
@@ -1478,7 +1517,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C33" s="13" t="n">
         <v>1</v>
@@ -1499,7 +1538,7 @@
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12"/>
       <c r="B34" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C34" s="13" t="n">
         <v>1</v>
@@ -1520,7 +1559,7 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12"/>
       <c r="B35" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C35" s="13" t="n">
         <v>1</v>
@@ -1540,7 +1579,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -1562,7 +1601,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C37" s="13" t="n">
         <v>1</v>
@@ -1585,7 +1624,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C38" s="13" t="n">
         <v>1</v>
@@ -1608,7 +1647,7 @@
         <v>3</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C39" s="13" t="n">
         <v>1</v>
@@ -1631,7 +1670,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C40" s="13" t="n">
         <v>1</v>
@@ -1652,7 +1691,7 @@
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="12"/>
       <c r="B41" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C41" s="13" t="n">
         <v>1</v>
@@ -1673,7 +1712,7 @@
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="12"/>
       <c r="B42" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C42" s="13" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
TDD: refactored entity constructors to one, which uses hashmap
</commit_message>
<xml_diff>
--- a/resources/Effects.xlsx
+++ b/resources/Effects.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="43">
   <si>
     <t xml:space="preserve">Effect</t>
   </si>
@@ -441,7 +441,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
+      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1690,7 +1690,9 @@
       <c r="C40" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D40" s="14"/>
+      <c r="D40" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
@@ -1711,7 +1713,9 @@
       <c r="C41" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D41" s="14"/>
+      <c r="D41" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
@@ -1732,7 +1736,9 @@
       <c r="C42" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D42" s="14"/>
+      <c r="D42" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>

</xml_diff>